<commit_message>
added import into the box table and the vials table
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luke/Uni/Professional Computing/CITS3200-repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AE75952-2F7E-7741-A379-DA2D0DFD969C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77D3049-E758-DA43-8591-92AEB88D166C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15320" xr2:uid="{16F4C9F6-C307-1F4D-87B6-4B73A910641B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="274">
   <si>
     <t>Box ID:</t>
   </si>
@@ -854,6 +854,9 @@
   </si>
   <si>
     <t>V10</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1254,7 @@
   <dimension ref="A1:Q227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1276,7 +1279,9 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
@@ -7025,16 +7030,78 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="D223:F223"/>
-    <mergeCell ref="D224:F224"/>
-    <mergeCell ref="D225:F225"/>
-    <mergeCell ref="D226:F226"/>
-    <mergeCell ref="D227:F227"/>
-    <mergeCell ref="D217:F217"/>
-    <mergeCell ref="D218:F218"/>
-    <mergeCell ref="D219:F219"/>
-    <mergeCell ref="D220:F220"/>
-    <mergeCell ref="D221:F221"/>
+    <mergeCell ref="D150:F150"/>
+    <mergeCell ref="D139:F139"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D145:F145"/>
+    <mergeCell ref="D146:F146"/>
+    <mergeCell ref="D147:F147"/>
+    <mergeCell ref="D148:F148"/>
+    <mergeCell ref="D149:F149"/>
+    <mergeCell ref="D162:F162"/>
+    <mergeCell ref="D151:F151"/>
+    <mergeCell ref="D152:F152"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="D154:F154"/>
+    <mergeCell ref="D155:F155"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="D157:F157"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="D159:F159"/>
+    <mergeCell ref="D160:F160"/>
+    <mergeCell ref="D161:F161"/>
+    <mergeCell ref="D174:F174"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="D164:F164"/>
+    <mergeCell ref="D165:F165"/>
+    <mergeCell ref="D166:F166"/>
+    <mergeCell ref="D167:F167"/>
+    <mergeCell ref="D168:F168"/>
+    <mergeCell ref="D169:F169"/>
+    <mergeCell ref="D170:F170"/>
+    <mergeCell ref="D171:F171"/>
+    <mergeCell ref="D172:F172"/>
+    <mergeCell ref="D173:F173"/>
+    <mergeCell ref="D186:F186"/>
+    <mergeCell ref="D175:F175"/>
+    <mergeCell ref="D176:F176"/>
+    <mergeCell ref="D177:F177"/>
+    <mergeCell ref="D178:F178"/>
+    <mergeCell ref="D179:F179"/>
+    <mergeCell ref="D180:F180"/>
+    <mergeCell ref="D181:F181"/>
+    <mergeCell ref="D182:F182"/>
+    <mergeCell ref="D183:F183"/>
+    <mergeCell ref="D184:F184"/>
+    <mergeCell ref="D185:F185"/>
+    <mergeCell ref="D198:F198"/>
+    <mergeCell ref="D187:F187"/>
+    <mergeCell ref="D188:F188"/>
+    <mergeCell ref="D189:F189"/>
+    <mergeCell ref="D190:F190"/>
+    <mergeCell ref="D191:F191"/>
+    <mergeCell ref="D192:F192"/>
+    <mergeCell ref="D193:F193"/>
+    <mergeCell ref="D194:F194"/>
+    <mergeCell ref="D195:F195"/>
+    <mergeCell ref="D196:F196"/>
+    <mergeCell ref="D197:F197"/>
+    <mergeCell ref="D210:F210"/>
+    <mergeCell ref="D199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D201:F201"/>
+    <mergeCell ref="D202:F202"/>
+    <mergeCell ref="D203:F203"/>
+    <mergeCell ref="D204:F204"/>
+    <mergeCell ref="D205:F205"/>
+    <mergeCell ref="D206:F206"/>
+    <mergeCell ref="D207:F207"/>
+    <mergeCell ref="D208:F208"/>
+    <mergeCell ref="D209:F209"/>
     <mergeCell ref="D222:F222"/>
     <mergeCell ref="D211:F211"/>
     <mergeCell ref="D212:F212"/>
@@ -7042,78 +7109,16 @@
     <mergeCell ref="D214:F214"/>
     <mergeCell ref="D215:F215"/>
     <mergeCell ref="D216:F216"/>
-    <mergeCell ref="D205:F205"/>
-    <mergeCell ref="D206:F206"/>
-    <mergeCell ref="D207:F207"/>
-    <mergeCell ref="D208:F208"/>
-    <mergeCell ref="D209:F209"/>
-    <mergeCell ref="D210:F210"/>
-    <mergeCell ref="D199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D201:F201"/>
-    <mergeCell ref="D202:F202"/>
-    <mergeCell ref="D203:F203"/>
-    <mergeCell ref="D204:F204"/>
-    <mergeCell ref="D193:F193"/>
-    <mergeCell ref="D194:F194"/>
-    <mergeCell ref="D195:F195"/>
-    <mergeCell ref="D196:F196"/>
-    <mergeCell ref="D197:F197"/>
-    <mergeCell ref="D198:F198"/>
-    <mergeCell ref="D187:F187"/>
-    <mergeCell ref="D188:F188"/>
-    <mergeCell ref="D189:F189"/>
-    <mergeCell ref="D190:F190"/>
-    <mergeCell ref="D191:F191"/>
-    <mergeCell ref="D192:F192"/>
-    <mergeCell ref="D181:F181"/>
-    <mergeCell ref="D182:F182"/>
-    <mergeCell ref="D183:F183"/>
-    <mergeCell ref="D184:F184"/>
-    <mergeCell ref="D185:F185"/>
-    <mergeCell ref="D186:F186"/>
-    <mergeCell ref="D175:F175"/>
-    <mergeCell ref="D176:F176"/>
-    <mergeCell ref="D177:F177"/>
-    <mergeCell ref="D178:F178"/>
-    <mergeCell ref="D179:F179"/>
-    <mergeCell ref="D180:F180"/>
-    <mergeCell ref="D169:F169"/>
-    <mergeCell ref="D170:F170"/>
-    <mergeCell ref="D171:F171"/>
-    <mergeCell ref="D172:F172"/>
-    <mergeCell ref="D173:F173"/>
-    <mergeCell ref="D174:F174"/>
-    <mergeCell ref="D163:F163"/>
-    <mergeCell ref="D164:F164"/>
-    <mergeCell ref="D165:F165"/>
-    <mergeCell ref="D166:F166"/>
-    <mergeCell ref="D167:F167"/>
-    <mergeCell ref="D168:F168"/>
-    <mergeCell ref="D157:F157"/>
-    <mergeCell ref="D158:F158"/>
-    <mergeCell ref="D159:F159"/>
-    <mergeCell ref="D160:F160"/>
-    <mergeCell ref="D161:F161"/>
-    <mergeCell ref="D162:F162"/>
-    <mergeCell ref="D151:F151"/>
-    <mergeCell ref="D152:F152"/>
-    <mergeCell ref="D153:F153"/>
-    <mergeCell ref="D154:F154"/>
-    <mergeCell ref="D155:F155"/>
-    <mergeCell ref="D156:F156"/>
-    <mergeCell ref="D145:F145"/>
-    <mergeCell ref="D146:F146"/>
-    <mergeCell ref="D147:F147"/>
-    <mergeCell ref="D148:F148"/>
-    <mergeCell ref="D149:F149"/>
-    <mergeCell ref="D150:F150"/>
-    <mergeCell ref="D139:F139"/>
-    <mergeCell ref="D140:F140"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="D142:F142"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D217:F217"/>
+    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="D219:F219"/>
+    <mergeCell ref="D220:F220"/>
+    <mergeCell ref="D221:F221"/>
+    <mergeCell ref="D223:F223"/>
+    <mergeCell ref="D224:F224"/>
+    <mergeCell ref="D225:F225"/>
+    <mergeCell ref="D226:F226"/>
+    <mergeCell ref="D227:F227"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>